<commit_message>
Add time estimate to each task.
</commit_message>
<xml_diff>
--- a/Scrum Files/product_backlog.xlsx
+++ b/Scrum Files/product_backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76DB09F-5E0C-4F99-97C9-02E36D19FFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B6F8BA-79D0-441C-B94C-A0E728A40971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="145">
   <si>
     <t>Task</t>
   </si>
@@ -405,6 +405,69 @@
   </si>
   <si>
     <t>Sprint Points</t>
+  </si>
+  <si>
+    <t>Time Estimate</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>2 hour</t>
+  </si>
+  <si>
+    <t>3 hour</t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>0.5 hours</t>
+  </si>
+  <si>
+    <t>0.2 hours</t>
+  </si>
+  <si>
+    <t>5 hours</t>
+  </si>
+  <si>
+    <t>1-2 hours</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>1-3 days</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>3-4 hours</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>4-5 hours</t>
+  </si>
+  <si>
+    <t>1 hours</t>
+  </si>
+  <si>
+    <t>5-4 hours</t>
+  </si>
+  <si>
+    <t>1-3 hours</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>4-6 hours</t>
   </si>
 </sst>
 </file>
@@ -831,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -845,7 +908,7 @@
     <col min="4" max="4" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,8 +921,11 @@
       <c r="D1" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -872,8 +938,11 @@
       <c r="D2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E2" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -886,8 +955,11 @@
       <c r="D3" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E3" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -900,8 +972,11 @@
       <c r="D4" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E4" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -914,8 +989,11 @@
       <c r="D5" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E5" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -928,8 +1006,11 @@
       <c r="D6" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E6" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -942,8 +1023,11 @@
       <c r="D7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E7" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -956,8 +1040,11 @@
       <c r="D8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E8" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -970,8 +1057,11 @@
       <c r="D9" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E9" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -984,8 +1074,11 @@
       <c r="D10" s="4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E10" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -998,8 +1091,11 @@
       <c r="D11" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E11" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1012,8 +1108,11 @@
       <c r="D12" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E12" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1026,8 +1125,11 @@
       <c r="D13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E13" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1040,8 +1142,11 @@
       <c r="D14" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E14" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1054,8 +1159,11 @@
       <c r="D15" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E15" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1068,8 +1176,11 @@
       <c r="D16" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E16" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -1082,8 +1193,11 @@
       <c r="D17" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E17" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -1096,8 +1210,11 @@
       <c r="D18" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E18" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -1110,8 +1227,11 @@
       <c r="D19" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E19" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1124,8 +1244,11 @@
       <c r="D20" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E20" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1138,8 +1261,11 @@
       <c r="D21" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E21" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
@@ -1152,8 +1278,11 @@
       <c r="D22" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E22" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
@@ -1166,8 +1295,11 @@
       <c r="D23" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E23" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
@@ -1180,8 +1312,11 @@
       <c r="D24" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E24" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
@@ -1194,8 +1329,11 @@
       <c r="D25" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E25" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
@@ -1208,8 +1346,11 @@
       <c r="D26" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E26" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -1222,8 +1363,11 @@
       <c r="D27" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E27" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -1236,8 +1380,11 @@
       <c r="D28" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E28" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
@@ -1250,8 +1397,11 @@
       <c r="D29" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E29" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
@@ -1264,8 +1414,11 @@
       <c r="D30" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E30" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
@@ -1278,8 +1431,11 @@
       <c r="D31" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E31" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
@@ -1292,8 +1448,11 @@
       <c r="D32" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E32" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
@@ -1306,8 +1465,11 @@
       <c r="D33" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E33" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
@@ -1320,8 +1482,11 @@
       <c r="D34" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E34" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
@@ -1334,8 +1499,11 @@
       <c r="D35" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E35" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
@@ -1348,8 +1516,11 @@
       <c r="D36" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E36" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>38</v>
       </c>
@@ -1362,8 +1533,11 @@
       <c r="D37" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E37" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
@@ -1376,8 +1550,11 @@
       <c r="D38" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E38" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>40</v>
       </c>
@@ -1390,8 +1567,11 @@
       <c r="D39" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E39" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
@@ -1404,8 +1584,11 @@
       <c r="D40" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E40" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
         <v>42</v>
       </c>
@@ -1418,8 +1601,11 @@
       <c r="D41" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E41" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>43</v>
       </c>
@@ -1432,8 +1618,11 @@
       <c r="D42" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E42" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
         <v>44</v>
       </c>
@@ -1446,8 +1635,11 @@
       <c r="D43" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E43" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>45</v>
       </c>
@@ -1460,8 +1652,11 @@
       <c r="D44" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E44" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
@@ -1474,8 +1669,11 @@
       <c r="D45" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E45" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
@@ -1488,8 +1686,11 @@
       <c r="D46" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E46" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
@@ -1502,8 +1703,11 @@
       <c r="D47" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E47" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
@@ -1516,8 +1720,11 @@
       <c r="D48" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E48" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
@@ -1530,8 +1737,11 @@
       <c r="D49" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E49" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
@@ -1544,8 +1754,11 @@
       <c r="D50" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E50" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
@@ -1558,8 +1771,11 @@
       <c r="D51" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E51" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
         <v>58</v>
       </c>
@@ -1572,8 +1788,11 @@
       <c r="D52" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E52" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
         <v>59</v>
       </c>
@@ -1586,8 +1805,11 @@
       <c r="D53" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E53" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
         <v>60</v>
       </c>
@@ -1600,8 +1822,11 @@
       <c r="D54" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E54" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
         <v>61</v>
       </c>
@@ -1614,8 +1839,11 @@
       <c r="D55" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E55" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
         <v>62</v>
       </c>
@@ -1628,8 +1856,11 @@
       <c r="D56" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E56" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
         <v>63</v>
       </c>
@@ -1642,8 +1873,11 @@
       <c r="D57" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E57" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
         <v>64</v>
       </c>
@@ -1656,8 +1890,11 @@
       <c r="D58" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E58" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>65</v>
       </c>
@@ -1670,8 +1907,11 @@
       <c r="D59" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E59" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
         <v>66</v>
       </c>
@@ -1684,8 +1924,11 @@
       <c r="D60" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E60" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
         <v>67</v>
       </c>
@@ -1698,8 +1941,11 @@
       <c r="D61" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E61" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
         <v>68</v>
       </c>
@@ -1712,8 +1958,11 @@
       <c r="D62" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E62" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
         <v>69</v>
       </c>
@@ -1726,8 +1975,11 @@
       <c r="D63" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E63" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
         <v>70</v>
       </c>
@@ -1740,8 +1992,11 @@
       <c r="D64" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E64" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
         <v>71</v>
       </c>
@@ -1754,8 +2009,11 @@
       <c r="D65" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E65" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="3" t="s">
         <v>72</v>
       </c>
@@ -1768,8 +2026,11 @@
       <c r="D66" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E66" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="3" t="s">
         <v>73</v>
       </c>
@@ -1782,8 +2043,11 @@
       <c r="D67" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E67" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="3" t="s">
         <v>74</v>
       </c>
@@ -1796,8 +2060,11 @@
       <c r="D68" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E68" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
         <v>75</v>
       </c>
@@ -1810,8 +2077,11 @@
       <c r="D69" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E69" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
         <v>76</v>
       </c>
@@ -1824,8 +2094,11 @@
       <c r="D70" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E70" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
         <v>77</v>
       </c>
@@ -1838,8 +2111,11 @@
       <c r="D71" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E71" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
         <v>78</v>
       </c>
@@ -1852,8 +2128,11 @@
       <c r="D72" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E72" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
         <v>79</v>
       </c>
@@ -1866,8 +2145,11 @@
       <c r="D73" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E73" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
         <v>80</v>
       </c>
@@ -1880,8 +2162,11 @@
       <c r="D74" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E74" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
         <v>81</v>
       </c>
@@ -1894,8 +2179,11 @@
       <c r="D75" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E75" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
         <v>82</v>
       </c>
@@ -1908,8 +2196,11 @@
       <c r="D76" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E76" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
         <v>83</v>
       </c>
@@ -1922,8 +2213,11 @@
       <c r="D77" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E77" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
         <v>84</v>
       </c>
@@ -1936,8 +2230,11 @@
       <c r="D78" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E78" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
         <v>85</v>
       </c>
@@ -1950,8 +2247,11 @@
       <c r="D79" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E79" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
         <v>86</v>
       </c>
@@ -1964,8 +2264,11 @@
       <c r="D80" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E80" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
         <v>87</v>
       </c>
@@ -1978,8 +2281,11 @@
       <c r="D81" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E81" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
         <v>88</v>
       </c>
@@ -1992,8 +2298,11 @@
       <c r="D82" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E82" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
         <v>89</v>
       </c>
@@ -2006,8 +2315,11 @@
       <c r="D83" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E83" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
         <v>90</v>
       </c>
@@ -2020,8 +2332,11 @@
       <c r="D84" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E84" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
         <v>91</v>
       </c>
@@ -2034,8 +2349,11 @@
       <c r="D85" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E85" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
         <v>92</v>
       </c>
@@ -2048,8 +2366,11 @@
       <c r="D86" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E86" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="3" t="s">
         <v>93</v>
       </c>
@@ -2062,8 +2383,11 @@
       <c r="D87" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E87" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="3" t="s">
         <v>94</v>
       </c>
@@ -2076,8 +2400,11 @@
       <c r="D88" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E88" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="3" t="s">
         <v>95</v>
       </c>
@@ -2090,8 +2417,11 @@
       <c r="D89" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E89" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="3" t="s">
         <v>96</v>
       </c>
@@ -2104,8 +2434,11 @@
       <c r="D90" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E90" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="3" t="s">
         <v>97</v>
       </c>
@@ -2118,8 +2451,11 @@
       <c r="D91" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E91" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="3" t="s">
         <v>98</v>
       </c>
@@ -2132,8 +2468,11 @@
       <c r="D92" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E92" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3" t="s">
         <v>99</v>
       </c>
@@ -2146,8 +2485,11 @@
       <c r="D93" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E93" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
         <v>100</v>
       </c>
@@ -2160,8 +2502,11 @@
       <c r="D94" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E94" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
         <v>101</v>
       </c>
@@ -2174,8 +2519,11 @@
       <c r="D95" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E95" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
         <v>102</v>
       </c>
@@ -2188,8 +2536,11 @@
       <c r="D96" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E96" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
         <v>103</v>
       </c>
@@ -2202,8 +2553,11 @@
       <c r="D97" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E97" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="3" t="s">
         <v>104</v>
       </c>
@@ -2216,8 +2570,11 @@
       <c r="D98" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E98" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="3" t="s">
         <v>105</v>
       </c>
@@ -2230,8 +2587,11 @@
       <c r="D99" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E99" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="3" t="s">
         <v>106</v>
       </c>
@@ -2244,8 +2604,11 @@
       <c r="D100" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E100" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="3" t="s">
         <v>107</v>
       </c>
@@ -2258,8 +2621,11 @@
       <c r="D101" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E101" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="3" t="s">
         <v>108</v>
       </c>
@@ -2272,8 +2638,11 @@
       <c r="D102" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E102" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3" t="s">
         <v>109</v>
       </c>
@@ -2286,8 +2655,11 @@
       <c r="D103" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E103" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="3" t="s">
         <v>110</v>
       </c>
@@ -2300,8 +2672,11 @@
       <c r="D104" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E104" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="3" t="s">
         <v>111</v>
       </c>
@@ -2314,8 +2689,11 @@
       <c r="D105" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E105" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="3" t="s">
         <v>112</v>
       </c>
@@ -2328,8 +2706,11 @@
       <c r="D106" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E106" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="3" t="s">
         <v>113</v>
       </c>
@@ -2342,8 +2723,11 @@
       <c r="D107" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E107" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3" t="s">
         <v>114</v>
       </c>
@@ -2356,8 +2740,11 @@
       <c r="D108" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E108" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="3" t="s">
         <v>115</v>
       </c>
@@ -2370,8 +2757,11 @@
       <c r="D109" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E109" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="3" t="s">
         <v>116</v>
       </c>
@@ -2384,8 +2774,11 @@
       <c r="D110" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E110" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="3" t="s">
         <v>117</v>
       </c>
@@ -2398,8 +2791,11 @@
       <c r="D111" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E111" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3" t="s">
         <v>118</v>
       </c>
@@ -2412,8 +2808,11 @@
       <c r="D112" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E112" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3" t="s">
         <v>119</v>
       </c>
@@ -2426,8 +2825,11 @@
       <c r="D113" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E113" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="3" t="s">
         <v>120</v>
       </c>
@@ -2440,8 +2842,11 @@
       <c r="D114" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E114" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="3" t="s">
         <v>121</v>
       </c>
@@ -2454,8 +2859,11 @@
       <c r="D115" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E115" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="3" t="s">
         <v>122</v>
       </c>
@@ -2468,8 +2876,11 @@
       <c r="D116" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E116" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D117">
         <f>SUM(D2:D116)</f>
         <v>291.2</v>

</xml_diff>

<commit_message>
Add dependencies to each product backlog task.
</commit_message>
<xml_diff>
--- a/Scrum Files/product_backlog.xlsx
+++ b/Scrum Files/product_backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B6F8BA-79D0-441C-B94C-A0E728A40971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487C5673-0A68-4665-8CDD-6C0B728DF34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="163">
   <si>
     <t>Task</t>
   </si>
@@ -468,6 +468,60 @@
   </si>
   <si>
     <t>4-6 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Diagram, </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Design Doc sections</t>
+  </si>
+  <si>
+    <t>Personas and User Stories, system diagram, interface diagram</t>
+  </si>
+  <si>
+    <t>Finalized Design Doc</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Backend Login</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Create an API endpoint that returns the menu item components with its ingredients</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Create Get Inventory API Endpoint</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Create Get Inventory API Endpoint, Create Add Inventory API Endpoint, Create Edit Inventory API Endpoint</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Create Delete Inventory API Endpoint</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Add Buttons to Trigger Add or Edit Mode</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Create Add Employee API Endpoint, Create Edit Employee API Endpoint</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Create Add Menu Item API Endpoint, Create Edit Menu Item API Endpoint</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Create Add Item Component API Endpoint, Create Edit Item Component API Endpoint</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Implement Backend API for Review Submission</t>
+  </si>
+  <si>
+    <t>Set up the starter back end code and Github repository, Add a text resizing feature on the main screen</t>
+  </si>
+  <si>
+    <t>Website completed</t>
+  </si>
+  <si>
+    <t>Dependencies</t>
   </si>
 </sst>
 </file>
@@ -894,21 +948,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection sqref="A1:F116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.1796875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" customWidth="1"/>
+    <col min="1" max="1" width="43" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,8 +979,11 @@
       <c r="E1" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F1" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -941,8 +999,11 @@
       <c r="E2" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F2" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -958,8 +1019,11 @@
       <c r="E3" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F3" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -975,8 +1039,11 @@
       <c r="E4" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F4" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -992,8 +1059,11 @@
       <c r="E5" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1009,8 +1079,11 @@
       <c r="E6" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F6" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1026,8 +1099,11 @@
       <c r="E7" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F7" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1043,8 +1119,11 @@
       <c r="E8" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1060,8 +1139,11 @@
       <c r="E9" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1077,8 +1159,11 @@
       <c r="E10" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F10" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1094,8 +1179,11 @@
       <c r="E11" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F11" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1111,8 +1199,11 @@
       <c r="E12" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1128,8 +1219,11 @@
       <c r="E13" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F13" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1145,8 +1239,11 @@
       <c r="E14" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F14" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1162,8 +1259,11 @@
       <c r="E15" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F15" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1179,8 +1279,11 @@
       <c r="E16" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -1196,8 +1299,11 @@
       <c r="E17" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F17" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -1213,8 +1319,11 @@
       <c r="E18" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F18" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -1230,8 +1339,11 @@
       <c r="E19" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1247,8 +1359,11 @@
       <c r="E20" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1264,8 +1379,11 @@
       <c r="E21" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F21" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
@@ -1281,8 +1399,11 @@
       <c r="E22" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F22" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
@@ -1298,8 +1419,11 @@
       <c r="E23" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F23" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
@@ -1315,8 +1439,11 @@
       <c r="E24" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F24" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
@@ -1332,8 +1459,11 @@
       <c r="E25" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F25" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
@@ -1349,8 +1479,11 @@
       <c r="E26" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F26" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -1366,8 +1499,11 @@
       <c r="E27" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F27" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -1383,8 +1519,11 @@
       <c r="E28" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F28" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
@@ -1400,8 +1539,11 @@
       <c r="E29" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F29" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
@@ -1417,8 +1559,11 @@
       <c r="E30" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F30" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
@@ -1434,8 +1579,11 @@
       <c r="E31" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F31" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
@@ -1451,8 +1599,11 @@
       <c r="E32" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F32" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
@@ -1468,8 +1619,11 @@
       <c r="E33" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F33" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
@@ -1485,8 +1639,11 @@
       <c r="E34" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F34" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
@@ -1502,8 +1659,11 @@
       <c r="E35" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F35" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
@@ -1519,8 +1679,11 @@
       <c r="E36" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F36" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>38</v>
       </c>
@@ -1536,8 +1699,11 @@
       <c r="E37" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F37" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
@@ -1553,8 +1719,11 @@
       <c r="E38" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F38" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>40</v>
       </c>
@@ -1570,8 +1739,11 @@
       <c r="E39" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F39" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
@@ -1587,8 +1759,11 @@
       <c r="E40" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F40" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
         <v>42</v>
       </c>
@@ -1604,8 +1779,11 @@
       <c r="E41" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F41" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>43</v>
       </c>
@@ -1621,8 +1799,11 @@
       <c r="E42" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F42" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
         <v>44</v>
       </c>
@@ -1638,8 +1819,11 @@
       <c r="E43" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F43" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>45</v>
       </c>
@@ -1655,8 +1839,11 @@
       <c r="E44" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F44" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
@@ -1672,8 +1859,11 @@
       <c r="E45" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F45" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
@@ -1689,8 +1879,11 @@
       <c r="E46" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F46" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
@@ -1706,8 +1899,11 @@
       <c r="E47" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F47" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
@@ -1723,8 +1919,11 @@
       <c r="E48" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F48" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
@@ -1740,8 +1939,11 @@
       <c r="E49" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F49" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
@@ -1757,8 +1959,11 @@
       <c r="E50" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F50" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
@@ -1774,8 +1979,11 @@
       <c r="E51" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F51" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
         <v>58</v>
       </c>
@@ -1791,8 +1999,11 @@
       <c r="E52" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F52" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
         <v>59</v>
       </c>
@@ -1808,8 +2019,11 @@
       <c r="E53" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F53" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
         <v>60</v>
       </c>
@@ -1825,8 +2039,11 @@
       <c r="E54" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F54" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
         <v>61</v>
       </c>
@@ -1842,8 +2059,11 @@
       <c r="E55" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F55" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
         <v>62</v>
       </c>
@@ -1859,8 +2079,11 @@
       <c r="E56" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F56" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
         <v>63</v>
       </c>
@@ -1876,8 +2099,11 @@
       <c r="E57" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F57" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
         <v>64</v>
       </c>
@@ -1893,8 +2119,11 @@
       <c r="E58" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F58" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>65</v>
       </c>
@@ -1910,8 +2139,11 @@
       <c r="E59" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F59" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
         <v>66</v>
       </c>
@@ -1927,8 +2159,11 @@
       <c r="E60" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F60" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
         <v>67</v>
       </c>
@@ -1944,8 +2179,11 @@
       <c r="E61" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F61" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
         <v>68</v>
       </c>
@@ -1961,8 +2199,11 @@
       <c r="E62" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F62" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
         <v>69</v>
       </c>
@@ -1978,8 +2219,11 @@
       <c r="E63" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F63" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
         <v>70</v>
       </c>
@@ -1995,8 +2239,11 @@
       <c r="E64" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F64" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
         <v>71</v>
       </c>
@@ -2012,8 +2259,11 @@
       <c r="E65" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F65" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="3" t="s">
         <v>72</v>
       </c>
@@ -2029,8 +2279,11 @@
       <c r="E66" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F66" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="3" t="s">
         <v>73</v>
       </c>
@@ -2046,8 +2299,11 @@
       <c r="E67" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F67" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="3" t="s">
         <v>74</v>
       </c>
@@ -2063,8 +2319,11 @@
       <c r="E68" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F68" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
         <v>75</v>
       </c>
@@ -2080,8 +2339,11 @@
       <c r="E69" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F69" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
         <v>76</v>
       </c>
@@ -2097,8 +2359,11 @@
       <c r="E70" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F70" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
         <v>77</v>
       </c>
@@ -2114,8 +2379,11 @@
       <c r="E71" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F71" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
         <v>78</v>
       </c>
@@ -2131,8 +2399,11 @@
       <c r="E72" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F72" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
         <v>79</v>
       </c>
@@ -2148,8 +2419,11 @@
       <c r="E73" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F73" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
         <v>80</v>
       </c>
@@ -2165,8 +2439,11 @@
       <c r="E74" s="3" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F74" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
         <v>81</v>
       </c>
@@ -2182,8 +2459,11 @@
       <c r="E75" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F75" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
         <v>82</v>
       </c>
@@ -2199,8 +2479,11 @@
       <c r="E76" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F76" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
         <v>83</v>
       </c>
@@ -2216,8 +2499,11 @@
       <c r="E77" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F77" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
         <v>84</v>
       </c>
@@ -2233,8 +2519,11 @@
       <c r="E78" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F78" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
         <v>85</v>
       </c>
@@ -2250,8 +2539,11 @@
       <c r="E79" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F79" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
         <v>86</v>
       </c>
@@ -2267,8 +2559,11 @@
       <c r="E80" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F80" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
         <v>87</v>
       </c>
@@ -2284,8 +2579,11 @@
       <c r="E81" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F81" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
         <v>88</v>
       </c>
@@ -2301,8 +2599,11 @@
       <c r="E82" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F82" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
         <v>89</v>
       </c>
@@ -2318,8 +2619,11 @@
       <c r="E83" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F83" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
         <v>90</v>
       </c>
@@ -2335,8 +2639,11 @@
       <c r="E84" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F84" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
         <v>91</v>
       </c>
@@ -2352,8 +2659,11 @@
       <c r="E85" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F85" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
         <v>92</v>
       </c>
@@ -2369,8 +2679,11 @@
       <c r="E86" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F86" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="3" t="s">
         <v>93</v>
       </c>
@@ -2386,8 +2699,11 @@
       <c r="E87" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F87" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="3" t="s">
         <v>94</v>
       </c>
@@ -2403,8 +2719,11 @@
       <c r="E88" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F88" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="3" t="s">
         <v>95</v>
       </c>
@@ -2420,8 +2739,11 @@
       <c r="E89" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F89" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="3" t="s">
         <v>96</v>
       </c>
@@ -2437,8 +2759,11 @@
       <c r="E90" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F90" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="3" t="s">
         <v>97</v>
       </c>
@@ -2454,8 +2779,11 @@
       <c r="E91" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F91" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="3" t="s">
         <v>98</v>
       </c>
@@ -2471,8 +2799,11 @@
       <c r="E92" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F92" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3" t="s">
         <v>99</v>
       </c>
@@ -2488,8 +2819,11 @@
       <c r="E93" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F93" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
         <v>100</v>
       </c>
@@ -2505,8 +2839,11 @@
       <c r="E94" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F94" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
         <v>101</v>
       </c>
@@ -2522,8 +2859,11 @@
       <c r="E95" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F95" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
         <v>102</v>
       </c>
@@ -2539,8 +2879,11 @@
       <c r="E96" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F96" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
         <v>103</v>
       </c>
@@ -2556,8 +2899,11 @@
       <c r="E97" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F97" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="3" t="s">
         <v>104</v>
       </c>
@@ -2573,8 +2919,11 @@
       <c r="E98" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F98" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="3" t="s">
         <v>105</v>
       </c>
@@ -2590,8 +2939,11 @@
       <c r="E99" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F99" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="3" t="s">
         <v>106</v>
       </c>
@@ -2607,8 +2959,11 @@
       <c r="E100" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F100" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="3" t="s">
         <v>107</v>
       </c>
@@ -2624,8 +2979,11 @@
       <c r="E101" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F101" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="3" t="s">
         <v>108</v>
       </c>
@@ -2641,8 +2999,11 @@
       <c r="E102" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F102" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3" t="s">
         <v>109</v>
       </c>
@@ -2658,8 +3019,11 @@
       <c r="E103" s="3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F103" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="3" t="s">
         <v>110</v>
       </c>
@@ -2675,8 +3039,11 @@
       <c r="E104" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F104" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="3" t="s">
         <v>111</v>
       </c>
@@ -2692,8 +3059,11 @@
       <c r="E105" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F105" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="3" t="s">
         <v>112</v>
       </c>
@@ -2709,8 +3079,11 @@
       <c r="E106" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F106" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="3" t="s">
         <v>113</v>
       </c>
@@ -2726,8 +3099,11 @@
       <c r="E107" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F107" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3" t="s">
         <v>114</v>
       </c>
@@ -2743,8 +3119,11 @@
       <c r="E108" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F108" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="3" t="s">
         <v>115</v>
       </c>
@@ -2760,8 +3139,11 @@
       <c r="E109" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F109" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="3" t="s">
         <v>116</v>
       </c>
@@ -2777,8 +3159,11 @@
       <c r="E110" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F110" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="3" t="s">
         <v>117</v>
       </c>
@@ -2794,8 +3179,11 @@
       <c r="E111" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F111" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3" t="s">
         <v>118</v>
       </c>
@@ -2811,8 +3199,11 @@
       <c r="E112" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F112" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3" t="s">
         <v>119</v>
       </c>
@@ -2828,8 +3219,11 @@
       <c r="E113" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F113" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="3" t="s">
         <v>120</v>
       </c>
@@ -2845,8 +3239,11 @@
       <c r="E114" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F114" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="3" t="s">
         <v>121</v>
       </c>
@@ -2862,8 +3259,11 @@
       <c r="E115" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F115" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="3" t="s">
         <v>122</v>
       </c>
@@ -2879,8 +3279,11 @@
       <c r="E116" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F116" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D117">
         <f>SUM(D2:D116)</f>
         <v>291.2</v>

</xml_diff>

<commit_message>
Update description of product backlog and scrum meeting dates.
</commit_message>
<xml_diff>
--- a/Scrum Files/product_backlog.xlsx
+++ b/Scrum Files/product_backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487C5673-0A68-4665-8CDD-6C0B728DF34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA26D231-41B6-4159-A0B7-FABFB9CB2316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -332,9 +332,6 @@
     <t>Integrate Google Translate API into the kiosk interface</t>
   </si>
   <si>
-    <t>Create a dropdown menu on the main screen for language selection</t>
-  </si>
-  <si>
     <t>Ensure all menu text, buttons, and labels dynamically update when a language is selected</t>
   </si>
   <si>
@@ -522,6 +519,9 @@
   </si>
   <si>
     <t>Dependencies</t>
+  </si>
+  <si>
+    <t>Create a dropdown menu on the landing pages and navigation bar for language selection</t>
   </si>
 </sst>
 </file>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection sqref="A1:F116"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -974,13 +974,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -997,10 +997,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1017,10 +1017,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1037,10 +1037,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1057,13 +1057,13 @@
         <v>4</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1077,10 +1077,10 @@
         <v>0.5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1097,10 +1097,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1117,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>12</v>
@@ -1137,7 +1137,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>12</v>
@@ -1157,10 +1157,10 @@
         <v>0.2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -1177,13 +1177,13 @@
         <v>5</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>0.5</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>12</v>
@@ -1217,10 +1217,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1237,10 +1237,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1257,7 +1257,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>6</v>
@@ -1277,7 +1277,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>6</v>
@@ -1297,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>17</v>
@@ -1317,7 +1317,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>15</v>
@@ -1337,7 +1337,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>16</v>
@@ -1357,7 +1357,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>19</v>
@@ -1377,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>24</v>
@@ -1397,10 +1397,10 @@
         <v>2</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1417,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>20</v>
@@ -1437,7 +1437,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>15</v>
@@ -1457,7 +1457,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>15</v>
@@ -1477,7 +1477,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>15</v>
@@ -1497,7 +1497,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>15</v>
@@ -1517,7 +1517,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>15</v>
@@ -1537,7 +1537,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>15</v>
@@ -1557,7 +1557,7 @@
         <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>15</v>
@@ -1577,7 +1577,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>15</v>
@@ -1597,10 +1597,10 @@
         <v>2</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -1617,10 +1617,10 @@
         <v>2</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -1637,10 +1637,10 @@
         <v>2</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -1657,10 +1657,10 @@
         <v>2</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -1677,10 +1677,10 @@
         <v>2</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
@@ -1697,10 +1697,10 @@
         <v>2</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1717,7 +1717,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>15</v>
@@ -1737,7 +1737,7 @@
         <v>5</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>15</v>
@@ -1757,7 +1757,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>15</v>
@@ -1777,7 +1777,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>15</v>
@@ -1797,10 +1797,10 @@
         <v>4</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1817,7 +1817,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>15</v>
@@ -1837,7 +1837,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>15</v>
@@ -1857,10 +1857,10 @@
         <v>2</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1877,7 +1877,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>15</v>
@@ -1897,7 +1897,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>15</v>
@@ -1917,7 +1917,7 @@
         <v>2</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>15</v>
@@ -1937,7 +1937,7 @@
         <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>15</v>
@@ -1957,7 +1957,7 @@
         <v>3</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>15</v>
@@ -1977,10 +1977,10 @@
         <v>2</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1997,7 +1997,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>15</v>
@@ -2017,10 +2017,10 @@
         <v>2</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2037,7 +2037,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>15</v>
@@ -2057,7 +2057,7 @@
         <v>4</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>15</v>
@@ -2077,7 +2077,7 @@
         <v>4</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>15</v>
@@ -2097,10 +2097,10 @@
         <v>2</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2117,7 +2117,7 @@
         <v>2</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>15</v>
@@ -2137,7 +2137,7 @@
         <v>2</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>15</v>
@@ -2157,7 +2157,7 @@
         <v>2</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>15</v>
@@ -2177,10 +2177,10 @@
         <v>2</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2197,7 +2197,7 @@
         <v>4</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>15</v>
@@ -2217,7 +2217,7 @@
         <v>4</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>15</v>
@@ -2237,7 +2237,7 @@
         <v>4</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>15</v>
@@ -2257,7 +2257,7 @@
         <v>2</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>15</v>
@@ -2277,7 +2277,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>15</v>
@@ -2297,10 +2297,10 @@
         <v>2</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2317,7 +2317,7 @@
         <v>4</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>15</v>
@@ -2337,7 +2337,7 @@
         <v>4</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>15</v>
@@ -2357,7 +2357,7 @@
         <v>4</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>15</v>
@@ -2377,10 +2377,10 @@
         <v>2</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2397,7 +2397,7 @@
         <v>2</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>15</v>
@@ -2417,7 +2417,7 @@
         <v>2</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>15</v>
@@ -2437,7 +2437,7 @@
         <v>5</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>15</v>
@@ -2457,7 +2457,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>15</v>
@@ -2477,7 +2477,7 @@
         <v>2</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>15</v>
@@ -2497,7 +2497,7 @@
         <v>2</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>15</v>
@@ -2517,10 +2517,10 @@
         <v>2</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2537,7 +2537,7 @@
         <v>3</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>15</v>
@@ -2557,7 +2557,7 @@
         <v>2</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>15</v>
@@ -2577,7 +2577,7 @@
         <v>5</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>15</v>
@@ -2597,7 +2597,7 @@
         <v>4</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>15</v>
@@ -2617,7 +2617,7 @@
         <v>2</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>15</v>
@@ -2637,7 +2637,7 @@
         <v>2</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>15</v>
@@ -2657,7 +2657,7 @@
         <v>2</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>15</v>
@@ -2677,7 +2677,7 @@
         <v>2</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>15</v>
@@ -2697,7 +2697,7 @@
         <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>15</v>
@@ -2717,7 +2717,7 @@
         <v>4</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>15</v>
@@ -2737,7 +2737,7 @@
         <v>4</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>15</v>
@@ -2757,7 +2757,7 @@
         <v>2</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>15</v>
@@ -2777,7 +2777,7 @@
         <v>2</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>15</v>
@@ -2797,7 +2797,7 @@
         <v>4</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F92" s="3" t="s">
         <v>15</v>
@@ -2805,7 +2805,7 @@
     </row>
     <row r="93" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>48</v>
@@ -2817,7 +2817,7 @@
         <v>2</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>15</v>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="94" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>48</v>
@@ -2837,7 +2837,7 @@
         <v>2</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>15</v>
@@ -2845,7 +2845,7 @@
     </row>
     <row r="95" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>48</v>
@@ -2857,7 +2857,7 @@
         <v>2</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>15</v>
@@ -2865,7 +2865,7 @@
     </row>
     <row r="96" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>48</v>
@@ -2877,7 +2877,7 @@
         <v>2</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>15</v>
@@ -2885,7 +2885,7 @@
     </row>
     <row r="97" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>48</v>
@@ -2897,7 +2897,7 @@
         <v>2</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>15</v>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="98" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>48</v>
@@ -2917,7 +2917,7 @@
         <v>2</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F98" s="3" t="s">
         <v>15</v>
@@ -2925,7 +2925,7 @@
     </row>
     <row r="99" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>48</v>
@@ -2937,7 +2937,7 @@
         <v>2</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F99" s="3" t="s">
         <v>15</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="100" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>48</v>
@@ -2957,7 +2957,7 @@
         <v>2</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>15</v>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="101" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>48</v>
@@ -2977,7 +2977,7 @@
         <v>2</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>15</v>
@@ -2985,7 +2985,7 @@
     </row>
     <row r="102" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>48</v>
@@ -2997,15 +2997,15 @@
         <v>2</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>48</v>
@@ -3017,7 +3017,7 @@
         <v>5</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>15</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="104" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>48</v>
@@ -3037,7 +3037,7 @@
         <v>2</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>15</v>
@@ -3045,7 +3045,7 @@
     </row>
     <row r="105" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>48</v>
@@ -3057,7 +3057,7 @@
         <v>2</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F105" s="3" t="s">
         <v>15</v>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="106" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>48</v>
@@ -3077,7 +3077,7 @@
         <v>2</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>15</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="107" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>48</v>
@@ -3097,7 +3097,7 @@
         <v>2</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>15</v>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="108" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>48</v>
@@ -3117,7 +3117,7 @@
         <v>2</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F108" s="3" t="s">
         <v>15</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="109" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>48</v>
@@ -3137,7 +3137,7 @@
         <v>2</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F109" s="3" t="s">
         <v>15</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="110" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>48</v>
@@ -3157,7 +3157,7 @@
         <v>2</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F110" s="3" t="s">
         <v>15</v>
@@ -3165,7 +3165,7 @@
     </row>
     <row r="111" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>48</v>
@@ -3177,7 +3177,7 @@
         <v>2</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F111" s="3" t="s">
         <v>15</v>
@@ -3185,7 +3185,7 @@
     </row>
     <row r="112" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>48</v>
@@ -3197,7 +3197,7 @@
         <v>2</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F112" s="3" t="s">
         <v>15</v>
@@ -3205,7 +3205,7 @@
     </row>
     <row r="113" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>48</v>
@@ -3217,7 +3217,7 @@
         <v>2</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>15</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="114" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>48</v>
@@ -3237,7 +3237,7 @@
         <v>2</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F114" s="3" t="s">
         <v>15</v>
@@ -3245,7 +3245,7 @@
     </row>
     <row r="115" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>48</v>
@@ -3257,7 +3257,7 @@
         <v>2</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F115" s="3" t="s">
         <v>15</v>
@@ -3265,7 +3265,7 @@
     </row>
     <row r="116" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>48</v>
@@ -3277,10 +3277,10 @@
         <v>2</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update sprint 3 materials for the github release.
</commit_message>
<xml_diff>
--- a/Scrum Files/product_backlog.xlsx
+++ b/Scrum Files/product_backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA26D231-41B6-4159-A0B7-FABFB9CB2316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1E9ACF-3221-4047-87A8-4164168FC639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -950,13 +950,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.36328125" style="5" customWidth="1"/>
     <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.08984375" bestFit="1" customWidth="1"/>
@@ -1063,7 +1063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
         <v>58</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
         <v>60</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>65</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
         <v>71</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
         <v>79</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
         <v>83</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
         <v>86</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
         <v>88</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3" t="s">
         <v>162</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
         <v>99</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
         <v>100</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
         <v>102</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="3" t="s">
         <v>104</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="3" t="s">
         <v>106</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3" t="s">
         <v>108</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="3" t="s">
         <v>114</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="3" t="s">
         <v>115</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3" t="s">
         <v>117</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3" t="s">
         <v>118</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="3" t="s">
         <v>121</v>
       </c>
@@ -3284,10 +3284,13 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D117">
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5">
         <f>SUM(D2:D116)</f>
         <v>291.2</v>
       </c>
+      <c r="E117" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update the last Sprint 3 materials.
</commit_message>
<xml_diff>
--- a/Scrum Files/product_backlog.xlsx
+++ b/Scrum Files/product_backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamda\Downloads\TAMU\Fall 2024\CSCE331\project-3-team-5b\Scrum Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1E9ACF-3221-4047-87A8-4164168FC639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41E38A5-4F0E-48D8-9EE2-C006A219826D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="162">
   <si>
     <t>Task</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Completed</t>
-  </si>
-  <si>
-    <t>Not Started</t>
   </si>
   <si>
     <t>High</t>
@@ -950,20 +947,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F117"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.36328125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.453125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -974,16 +971,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -991,19 +988,19 @@
         <v>47</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1011,19 +1008,19 @@
         <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1031,19 +1028,19 @@
         <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1051,19 +1048,19 @@
         <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="4">
         <v>4</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1071,19 +1068,19 @@
         <v>47</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="4">
         <v>0.5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1091,19 +1088,19 @@
         <v>47</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1111,19 +1108,19 @@
         <v>47</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1131,19 +1128,19 @@
         <v>47</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="4">
         <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1151,19 +1148,19 @@
         <v>47</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="4">
         <v>0.2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1171,19 +1168,19 @@
         <v>47</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="4">
         <v>5</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1191,19 +1188,19 @@
         <v>47</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="4">
         <v>0.5</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1211,19 +1208,19 @@
         <v>47</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1231,19 +1228,19 @@
         <v>47</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1251,19 +1248,19 @@
         <v>47</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="4">
         <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1271,19 +1268,19 @@
         <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="4">
         <v>5</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -1291,39 +1288,39 @@
         <v>47</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4">
         <v>2</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" s="4">
         <v>2</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -1331,19 +1328,19 @@
         <v>47</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="4">
         <v>2</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1351,19 +1348,19 @@
         <v>47</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1371,39 +1368,39 @@
         <v>47</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="4">
         <v>2</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="4">
         <v>2</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
@@ -1411,19 +1408,19 @@
         <v>47</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="4">
         <v>2</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
@@ -1431,19 +1428,19 @@
         <v>47</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="4">
         <v>2</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
@@ -1451,19 +1448,19 @@
         <v>47</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="4">
         <v>2</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
@@ -1471,19 +1468,19 @@
         <v>47</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="4">
         <v>2</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -1491,19 +1488,19 @@
         <v>47</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="4">
         <v>2</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -1511,19 +1508,19 @@
         <v>47</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="4">
         <v>1</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
@@ -1531,1759 +1528,1759 @@
         <v>47</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" s="4">
         <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="4">
         <v>2</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32" s="4">
         <v>2</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D33" s="4">
         <v>2</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" s="4">
         <v>2</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D35" s="4">
         <v>2</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="4">
         <v>2</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" s="4">
         <v>2</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D38" s="4">
         <v>3</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D39" s="4">
         <v>5</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D40" s="4">
         <v>2</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D41" s="4">
         <v>4</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" s="4">
         <v>4</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D43" s="4">
         <v>2</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D44" s="4">
         <v>4</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D45" s="4">
         <v>2</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="4">
+        <v>2</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="4" t="s">
+      <c r="B47" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="4">
+        <v>2</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="4">
-        <v>2</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="4">
-        <v>2</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="3" t="s">
+      <c r="D48" s="4">
+        <v>2</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" s="4">
-        <v>2</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="B49" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D49" s="4">
         <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="4">
         <v>3</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" s="4">
+        <v>2</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="4">
-        <v>2</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F51" s="3" t="s">
+      <c r="B52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" s="4">
+        <v>2</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" s="4">
+        <v>2</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="4">
-        <v>2</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="3" t="s">
+    <row r="54" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D53" s="4">
-        <v>2</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="B54" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D54" s="4">
         <v>1</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D55" s="4">
         <v>4</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D56" s="4">
         <v>4</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:6" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D57" s="4">
+        <v>2</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D57" s="4">
-        <v>2</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F57" s="3" t="s">
+      <c r="B58" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" s="4">
+        <v>2</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" s="4">
+        <v>2</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D60" s="4">
+        <v>2</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D61" s="4">
+        <v>2</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D58" s="4">
-        <v>2</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D59" s="4">
-        <v>2</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D60" s="4">
-        <v>2</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="3" t="s">
+    <row r="62" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D61" s="4">
-        <v>2</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="B62" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D62" s="4">
         <v>4</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D63" s="4">
         <v>4</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D64" s="4">
         <v>4</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D65" s="4">
+        <v>2</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D65" s="4">
-        <v>2</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="3" t="s">
+      <c r="B66" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D66" s="4">
+        <v>2</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D66" s="4">
-        <v>2</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="3" t="s">
+      <c r="B67" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D67" s="4">
+        <v>2</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D67" s="4">
-        <v>2</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="B68" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D68" s="4">
         <v>4</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D69" s="4">
         <v>4</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D70" s="4">
         <v>4</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:6" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D71" s="4">
+        <v>2</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D71" s="4">
-        <v>2</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="3" t="s">
+      <c r="B72" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="4">
+        <v>2</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D72" s="4">
-        <v>2</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="3" t="s">
+      <c r="B73" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D73" s="4">
+        <v>2</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D73" s="4">
-        <v>2</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="B74" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D74" s="4">
         <v>5</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D75" s="4">
+        <v>2</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B75" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D75" s="4">
-        <v>2</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="3" t="s">
+      <c r="B76" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D76" s="4">
+        <v>2</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D76" s="4">
-        <v>2</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="3" t="s">
+      <c r="B77" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D77" s="4">
+        <v>2</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D77" s="4">
-        <v>2</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="3" t="s">
+      <c r="B78" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D78" s="4">
+        <v>2</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B78" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D78" s="4">
-        <v>2</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="B79" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D79" s="4">
         <v>3</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D80" s="4">
+        <v>2</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D80" s="4">
-        <v>2</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="B81" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D81" s="4">
         <v>5</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D82" s="4">
         <v>4</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D83" s="4">
+        <v>2</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B83" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D83" s="4">
-        <v>2</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="3" t="s">
+      <c r="B84" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D84" s="4">
+        <v>2</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B84" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D84" s="4">
-        <v>2</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="3" t="s">
+      <c r="B85" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D85" s="4">
+        <v>2</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D85" s="4">
-        <v>2</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="3" t="s">
+      <c r="B86" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D86" s="4">
+        <v>2</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B86" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D86" s="4">
-        <v>2</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="B87" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D87" s="4">
         <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D88" s="4">
         <v>4</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D89" s="4">
         <v>4</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D90" s="4">
+        <v>2</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B90" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D90" s="4">
-        <v>2</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="3" t="s">
+      <c r="B91" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D91" s="4">
+        <v>2</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D91" s="4">
-        <v>2</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="B92" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D92" s="4">
         <v>4</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F92" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D93" s="4">
         <v>2</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D94" s="4">
+        <v>2</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B94" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D94" s="4">
-        <v>2</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="3" t="s">
+      <c r="B95" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D95" s="4">
+        <v>2</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B95" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D95" s="4">
-        <v>2</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="3" t="s">
+      <c r="B96" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D96" s="4">
+        <v>2</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B96" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D96" s="4">
-        <v>2</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="3" t="s">
+      <c r="B97" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D97" s="4">
+        <v>2</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B97" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D97" s="4">
-        <v>2</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="3" t="s">
+      <c r="B98" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D98" s="4">
+        <v>2</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B98" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D98" s="4">
-        <v>2</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="3" t="s">
+      <c r="B99" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D99" s="4">
+        <v>2</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B99" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D99" s="4">
-        <v>2</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="3" t="s">
+      <c r="B100" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D100" s="4">
+        <v>2</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B100" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D100" s="4">
-        <v>2</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="3" t="s">
+      <c r="B101" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D101" s="4">
+        <v>2</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B101" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D101" s="4">
-        <v>2</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="3" t="s">
+      <c r="B102" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D102" s="4">
+        <v>2</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B102" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D102" s="4">
-        <v>2</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="B103" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D103" s="4">
         <v>5</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D104" s="4">
+        <v>2</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D104" s="4">
-        <v>2</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="3" t="s">
+      <c r="B105" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D105" s="4">
+        <v>2</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D105" s="4">
-        <v>2</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="3" t="s">
+      <c r="B106" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D106" s="4">
+        <v>2</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D106" s="4">
-        <v>2</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="3" t="s">
+      <c r="B107" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D107" s="4">
+        <v>2</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B107" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D107" s="4">
-        <v>2</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F107" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="3" t="s">
+      <c r="B108" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D108" s="4">
+        <v>2</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B108" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D108" s="4">
-        <v>2</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F108" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="3" t="s">
+      <c r="B109" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D109" s="4">
+        <v>2</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B109" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D109" s="4">
-        <v>2</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="3" t="s">
+      <c r="B110" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D110" s="4">
+        <v>2</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B110" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D110" s="4">
-        <v>2</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F110" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="3" t="s">
+      <c r="B111" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D111" s="4">
+        <v>2</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B111" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D111" s="4">
-        <v>2</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="3" t="s">
+      <c r="B112" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D112" s="4">
+        <v>2</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B112" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D112" s="4">
-        <v>2</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="3" t="s">
+      <c r="B113" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D113" s="4">
+        <v>2</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B113" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D113" s="4">
-        <v>2</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="3" t="s">
+      <c r="B114" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D114" s="4">
+        <v>2</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B114" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D114" s="4">
-        <v>2</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F114" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="3" t="s">
+      <c r="B115" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D115" s="4">
+        <v>2</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B115" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D115" s="4">
-        <v>2</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A116" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="B116" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D116" s="4">
         <v>2</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5">

</xml_diff>